<commit_message>
changed some of the files in the dataset
</commit_message>
<xml_diff>
--- a/Dataset/LUFY/Benjamin/Session1/Annotator0.xlsx
+++ b/Dataset/LUFY/Benjamin/Session1/Annotator0.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>my favorite subject is accounting, its fun. my life at kyoto university has been great so far!</t>
+          <t>my favorite subject is accounting, its fun. my life at Doshisha Universityversity has been great so far!</t>
         </is>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>What does Benjamin study at kyoto university?</t>
+          <t>What does Benjamin study at Doshisha Universityversity?</t>
         </is>
       </c>
     </row>

</xml_diff>